<commit_message>
Update Leave Card 3/28/2023 1:12 PM
</commit_message>
<xml_diff>
--- a/REGULAR/TOLENTINO, ABRAHAM N.xlsx
+++ b/REGULAR/TOLENTINO, ABRAHAM N.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVECARD\REGULAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF26044-477E-4ADB-B7C5-4D8557ACE866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736D4957-BCA2-4C9D-AD01-A8F1763CAED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2C4B9B69-0AD3-46D4-A495-D1BDE1D16EC6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="76">
   <si>
     <t>PERIOD</t>
   </si>
@@ -256,6 +256,12 @@
   </si>
   <si>
     <t>BALI INDONESIA 4/29 - 5/1</t>
+  </si>
+  <si>
+    <t>BANGKOK THAILAND 7-9 2023</t>
+  </si>
+  <si>
+    <t>BANGKOK THAILAND 7-9 2024</t>
   </si>
 </sst>
 </file>
@@ -938,7 +944,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -1287,9 +1293,9 @@
   <dimension ref="A2:K137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3576" topLeftCell="A14" activePane="bottomLeft"/>
+      <pane ySplit="3576" topLeftCell="A19" activePane="bottomLeft"/>
       <selection activeCell="F2" sqref="F2:G2"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1456,7 +1462,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -1466,7 +1472,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>8.75</v>
+        <v>10</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -1630,7 +1636,7 @@
       </c>
       <c r="E16" s="9">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="F16" s="20">
         <v>4</v>
@@ -1642,7 +1648,7 @@
       <c r="H16" s="39"/>
       <c r="I16" s="9">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>8.75</v>
+        <v>10</v>
       </c>
       <c r="J16" s="11"/>
       <c r="K16" s="48" t="s">
@@ -1895,19 +1901,27 @@
       <c r="A28" s="40">
         <v>44986</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="39"/>
+      <c r="B28" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D28" s="39">
+        <v>1</v>
+      </c>
       <c r="E28" s="9"/>
       <c r="F28" s="20"/>
-      <c r="G28" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G28" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H28" s="39"/>
       <c r="I28" s="9"/>
       <c r="J28" s="11"/>
-      <c r="K28" s="20"/>
+      <c r="K28" s="20" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="40">

</xml_diff>